<commit_message>
Updated file in folder
Updates
</commit_message>
<xml_diff>
--- a/Classification evaluation/results/repeated_evaluation/repeated evaluation results.xlsx
+++ b/Classification evaluation/results/repeated_evaluation/repeated evaluation results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook-iscom/Documents/GitHub/AntiPhish-LLM/Classification evaluation/results/repeated_evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1760F4AC-C7E1-E643-AF59-5603904E8F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A776606-106F-294D-8CB9-180046A9305C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37040" yWindow="2520" windowWidth="22760" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="27040" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1318,83 +1318,83 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="97" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="25" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="70" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="71" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="75" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="79" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="47" xfId="99" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="75" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="41" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="25" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="79" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="71" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="72" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="70" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="34" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="29" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="100">
@@ -1812,7 +1812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A86" sqref="A86:XFD91"/>
     </sheetView>
   </sheetViews>
@@ -1834,17 +1834,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
       <c r="A5" s="4" t="s">
@@ -1852,46 +1852,46 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" customHeight="1">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="76" t="s">
+      <c r="C6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="76"/>
-      <c r="H6" s="76" t="s">
+      <c r="G6" s="72"/>
+      <c r="H6" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="74" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="90"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="75"/>
     </row>
     <row r="8" spans="1:9" ht="19" customHeight="1">
       <c r="A8" s="7" t="s">
@@ -2068,20 +2068,20 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="24" customHeight="1">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="71"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
     </row>
     <row r="16" spans="1:9" ht="34" customHeight="1">
-      <c r="A16" s="88" t="s">
+      <c r="A16" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="89"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="25" t="s">
         <v>20</v>
       </c>
@@ -2152,7 +2152,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19" customHeight="1">
-      <c r="A20" s="81"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
@@ -2170,14 +2170,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="24" customHeight="1">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="71"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1">
       <c r="A23" s="4" t="s">
@@ -2255,31 +2255,31 @@
       <c r="F27" s="44"/>
     </row>
     <row r="29" spans="1:6" ht="27" customHeight="1">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="71"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="67"/>
     </row>
     <row r="30" spans="1:6" ht="18" customHeight="1">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="86"/>
-      <c r="C30" s="74" t="s">
+      <c r="B30" s="82"/>
+      <c r="C30" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="76" t="s">
+      <c r="D30" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="77"/>
+      <c r="E30" s="74"/>
     </row>
     <row r="31" spans="1:6" ht="18" customHeight="1">
       <c r="A31" s="83"/>
       <c r="B31" s="84"/>
-      <c r="C31" s="75"/>
+      <c r="C31" s="71"/>
       <c r="D31" s="5" t="s">
         <v>38</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="19" customHeight="1">
-      <c r="A32" s="87" t="s">
+      <c r="A32" s="85" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="28" t="s">
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="35" customHeight="1">
-      <c r="A35" s="81"/>
+      <c r="A35" s="80"/>
       <c r="B35" s="3" t="s">
         <v>43</v>
       </c>
@@ -2350,13 +2350,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="35" customHeight="1">
-      <c r="A36" s="65" t="s">
+      <c r="A36" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="68"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="87"/>
+      <c r="E36" s="88"/>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="1" t="s">
@@ -2364,15 +2364,15 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="24" customHeight="1">
-      <c r="A41" s="69" t="s">
+      <c r="A41" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="70"/>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="71"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="67"/>
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1">
       <c r="A42" s="4" t="s">
@@ -2388,32 +2388,32 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="24" customHeight="1">
-      <c r="A44" s="82" t="s">
+      <c r="A44" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="74" t="s">
+      <c r="C44" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="76" t="s">
+      <c r="D44" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="76" t="s">
+      <c r="E44" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="F44" s="76" t="s">
+      <c r="F44" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="G44" s="77"/>
+      <c r="G44" s="74"/>
     </row>
     <row r="45" spans="1:7" ht="24" customHeight="1">
       <c r="A45" s="83"/>
       <c r="B45" s="84"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
       <c r="F45" s="5" t="s">
         <v>11</v>
       </c>
@@ -2487,7 +2487,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" customHeight="1">
-      <c r="A49" s="80"/>
+      <c r="A49" s="89"/>
       <c r="B49" s="47" t="s">
         <v>17</v>
       </c>
@@ -2508,7 +2508,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="19" customHeight="1">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="89" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" customHeight="1">
-      <c r="A53" s="80"/>
+      <c r="A53" s="89"/>
       <c r="B53" s="47" t="s">
         <v>17</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="21" customHeight="1">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="89" t="s">
         <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2659,7 +2659,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="21" customHeight="1">
-      <c r="A57" s="80"/>
+      <c r="A57" s="89"/>
       <c r="B57" s="47" t="s">
         <v>17</v>
       </c>
@@ -2680,7 +2680,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="19" customHeight="1">
-      <c r="A58" s="80" t="s">
+      <c r="A58" s="89" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2745,7 +2745,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="19" customHeight="1">
-      <c r="A61" s="80"/>
+      <c r="A61" s="89"/>
       <c r="B61" s="47" t="s">
         <v>17</v>
       </c>
@@ -2766,7 +2766,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="19" customHeight="1">
-      <c r="A62" s="80" t="s">
+      <c r="A62" s="89" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2831,7 +2831,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="19" customHeight="1">
-      <c r="A65" s="81"/>
+      <c r="A65" s="80"/>
       <c r="B65" s="3" t="s">
         <v>16</v>
       </c>
@@ -2852,15 +2852,15 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="19" customHeight="1">
-      <c r="A66" s="65" t="s">
+      <c r="A66" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="67"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
-      <c r="E66" s="67"/>
-      <c r="F66" s="67"/>
-      <c r="G66" s="68"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="87"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="87"/>
+      <c r="F66" s="87"/>
+      <c r="G66" s="88"/>
     </row>
     <row r="69" spans="1:7" ht="18">
       <c r="A69" s="1" t="s">
@@ -2868,12 +2868,12 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="24" customHeight="1">
-      <c r="A71" s="69" t="s">
+      <c r="A71" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="70"/>
-      <c r="C71" s="70"/>
-      <c r="D71" s="71"/>
+      <c r="B71" s="66"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="67"/>
     </row>
     <row r="72" spans="1:7" ht="18" customHeight="1">
       <c r="A72" s="4" t="s">
@@ -2881,20 +2881,20 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="18" customHeight="1">
-      <c r="A73" s="72" t="s">
+      <c r="A73" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="B73" s="74" t="s">
+      <c r="B73" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="76" t="s">
+      <c r="C73" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="D73" s="77"/>
+      <c r="D73" s="74"/>
     </row>
     <row r="74" spans="1:7" ht="18" customHeight="1">
-      <c r="A74" s="73"/>
-      <c r="B74" s="75"/>
+      <c r="A74" s="69"/>
+      <c r="B74" s="71"/>
       <c r="C74" s="61" t="s">
         <v>65</v>
       </c>
@@ -2975,31 +2975,61 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="32" customHeight="1">
-      <c r="A81" s="65" t="s">
+      <c r="A81" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="B81" s="65"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="66"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="90"/>
     </row>
     <row r="82" spans="1:4" ht="35" customHeight="1">
-      <c r="A82" s="65" t="s">
+      <c r="A82" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="66"/>
+      <c r="B82" s="86"/>
+      <c r="C82" s="86"/>
+      <c r="D82" s="90"/>
     </row>
     <row r="83" spans="1:4" ht="55" customHeight="1">
-      <c r="A83" s="65" t="s">
+      <c r="A83" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="B83" s="67"/>
-      <c r="C83" s="67"/>
-      <c r="D83" s="68"/>
+      <c r="B83" s="87"/>
+      <c r="C83" s="87"/>
+      <c r="D83" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -3009,36 +3039,6 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="A46:A49"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:D73"/>
   </mergeCells>
   <conditionalFormatting sqref="E46:E65">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
@@ -3050,15 +3050,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C2B6B18EE849BD448B8379240F5E7FFC" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="984de827d804d5bdf7b489642ab0f85d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30ccf00c-47aa-41f4-bd60-1bde55849fc9" xmlns:ns3="80e4ee34-ad22-48e2-8882-71f8157f78b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9461bd76d322c7b6dcd97a990b5ac799" ns2:_="" ns3:_="">
     <xsd:import namespace="30ccf00c-47aa-41f4-bd60-1bde55849fc9"/>
@@ -3287,15 +3278,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C934C9A-7C8E-4DF3-B563-068D781D64E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{061682F0-EB75-47A1-8C6D-5E1205BA3965}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3312,4 +3304,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C934C9A-7C8E-4DF3-B563-068D781D64E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>